<commit_message>
Problem 4 done, moving to Problem 5
</commit_message>
<xml_diff>
--- a/Assignment2_workbook.xlsx
+++ b/Assignment2_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\!MACHINE_LEARNING\CS4342_HW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdhm8\Documents\ML_HW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EEA0D2E-5E39-4C10-868E-7AFF7E60870E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5232FAFA-983E-4C7D-826C-104FDF4E629C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="2040" windowWidth="15410" windowHeight="15890" xr2:uid="{B362285D-7BBF-4426-AD6B-E61315AC3821}"/>
+    <workbookView xWindow="912" yWindow="7692" windowWidth="18984" windowHeight="9396" xr2:uid="{B362285D-7BBF-4426-AD6B-E61315AC3821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>sum Xi i to N:</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Has disease</t>
+  </si>
+  <si>
+    <t>Class1 prob</t>
+  </si>
+  <si>
+    <t>Class2 prob</t>
+  </si>
+  <si>
+    <t>Class3 prob</t>
   </si>
 </sst>
 </file>
@@ -1376,19 +1385,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B449F60B-47C0-4A15-A801-710204B9CBC2}">
-  <dimension ref="B2:D135"/>
+  <dimension ref="B2:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1396,31 +1406,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
         <v>7.89</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>-3.6</v>
       </c>
       <c r="C4">
         <v>-16.55</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2.2000000000000002</v>
       </c>
       <c r="C5">
         <v>6.73</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4.9000000000000004</v>
       </c>
@@ -1428,7 +1447,7 @@
         <v>17.91</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1.5</v>
       </c>
@@ -1436,7 +1455,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>3.1</v>
       </c>
@@ -1444,7 +1463,7 @@
         <v>12.84</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2.2000000000000002</v>
       </c>
@@ -1452,7 +1471,7 @@
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>-0.9</v>
       </c>
@@ -1460,7 +1479,7 @@
         <v>-5.35</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0.9</v>
       </c>
@@ -1468,7 +1487,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>-2.4</v>
       </c>
@@ -1476,7 +1495,7 @@
         <v>-12.31</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -1485,7 +1504,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1494,7 +1513,7 @@
         <v>25.319999999999993</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -1503,7 +1522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>6</v>
       </c>
@@ -1512,7 +1531,7 @@
         <v>2.5574747075655799</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -1521,7 +1540,7 @@
         <v>-1.0003951007506915E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -1530,7 +1549,7 @@
         <v>4.0031614304451202E-7</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>8</v>
       </c>
@@ -1538,13 +1557,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28">
         <f>1/SQRT(2*PI()*C24)*EXP(-(C3-(C21*B3+C22))^2/2*C24)</f>
         <v>630.53497864999463</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>10</v>
       </c>
@@ -1555,7 +1574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>1</v>
       </c>
@@ -1566,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>1</v>
       </c>
@@ -1577,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>1</v>
       </c>
@@ -1588,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>1</v>
       </c>
@@ -1599,7 +1618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>1</v>
       </c>
@@ -1610,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>1</v>
       </c>
@@ -1621,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>0</v>
       </c>
@@ -1632,7 +1651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>1</v>
       </c>
@@ -1643,7 +1662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>0</v>
       </c>
@@ -1654,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>1</v>
       </c>
@@ -1665,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>0</v>
       </c>
@@ -1676,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>1</v>
       </c>
@@ -1687,7 +1706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>0</v>
       </c>
@@ -1698,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>0</v>
       </c>
@@ -1709,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>0</v>
       </c>
@@ -1720,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>0</v>
       </c>
@@ -1731,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>1</v>
       </c>
@@ -1742,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>1</v>
       </c>
@@ -1753,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>1</v>
       </c>
@@ -1764,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>1</v>
       </c>
@@ -1775,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>0</v>
       </c>
@@ -1786,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>1</v>
       </c>
@@ -1797,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>1</v>
       </c>
@@ -1808,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59">
         <v>1</v>
       </c>
@@ -1819,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60">
         <v>1</v>
       </c>
@@ -1830,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>0</v>
       </c>
@@ -1841,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>1</v>
       </c>
@@ -1852,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>1</v>
       </c>
@@ -1863,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>0</v>
       </c>
@@ -1874,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>1</v>
       </c>
@@ -1885,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>0</v>
       </c>
@@ -1896,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67">
         <v>0</v>
       </c>
@@ -1907,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>0</v>
       </c>
@@ -1918,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>0</v>
       </c>
@@ -1929,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>1</v>
       </c>
@@ -1940,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71">
         <v>1</v>
       </c>
@@ -1951,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>1</v>
       </c>
@@ -1962,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73">
         <v>1</v>
       </c>
@@ -1973,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74">
         <v>1</v>
       </c>
@@ -1984,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75">
         <v>0</v>
       </c>
@@ -1995,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76">
         <v>1</v>
       </c>
@@ -2006,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77">
         <v>0</v>
       </c>
@@ -2017,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78">
         <v>1</v>
       </c>
@@ -2028,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79">
         <v>1</v>
       </c>
@@ -2039,7 +2058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>0</v>
       </c>
@@ -2050,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B81">
         <v>1</v>
       </c>
@@ -2061,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82">
         <v>1</v>
       </c>
@@ -2072,7 +2091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>1</v>
       </c>
@@ -2083,7 +2102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84">
         <v>0</v>
       </c>
@@ -2094,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85">
         <v>0</v>
       </c>
@@ -2105,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86">
         <v>1</v>
       </c>
@@ -2116,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87">
         <v>1</v>
       </c>
@@ -2127,7 +2146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88">
         <v>0</v>
       </c>
@@ -2138,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B89">
         <v>1</v>
       </c>
@@ -2149,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B90">
         <v>0</v>
       </c>
@@ -2160,7 +2179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B91">
         <v>0</v>
       </c>
@@ -2171,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B92">
         <v>1</v>
       </c>
@@ -2182,7 +2201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93">
         <v>0</v>
       </c>
@@ -2193,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94">
         <v>1</v>
       </c>
@@ -2204,7 +2223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B95">
         <v>1</v>
       </c>
@@ -2215,7 +2234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B96">
         <v>1</v>
       </c>
@@ -2226,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97">
         <v>0</v>
       </c>
@@ -2237,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98">
         <v>1</v>
       </c>
@@ -2248,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99">
         <v>1</v>
       </c>
@@ -2259,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100">
         <v>0</v>
       </c>
@@ -2270,7 +2289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101">
         <v>1</v>
       </c>
@@ -2281,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102">
         <v>0</v>
       </c>
@@ -2292,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103">
         <v>1</v>
       </c>
@@ -2303,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104">
         <v>0</v>
       </c>
@@ -2314,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105">
         <v>1</v>
       </c>
@@ -2325,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B106">
         <v>1</v>
       </c>
@@ -2336,7 +2355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B107">
         <v>1</v>
       </c>
@@ -2347,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B108">
         <v>1</v>
       </c>
@@ -2358,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B109">
         <v>1</v>
       </c>
@@ -2369,7 +2388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B110">
         <v>1</v>
       </c>
@@ -2380,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B111">
         <v>1</v>
       </c>
@@ -2391,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112">
         <v>0</v>
       </c>
@@ -2402,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B113">
         <v>1</v>
       </c>
@@ -2413,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B114">
         <v>0</v>
       </c>
@@ -2424,7 +2443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B115">
         <v>0</v>
       </c>
@@ -2435,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B116">
         <v>1</v>
       </c>
@@ -2446,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B117">
         <v>1</v>
       </c>
@@ -2457,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B118">
         <v>1</v>
       </c>
@@ -2468,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B119">
         <v>0</v>
       </c>
@@ -2479,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B120">
         <v>0</v>
       </c>
@@ -2490,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B121">
         <v>0</v>
       </c>
@@ -2501,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B122">
         <v>0</v>
       </c>
@@ -2512,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B123">
         <v>1</v>
       </c>
@@ -2523,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B124">
         <v>0</v>
       </c>
@@ -2534,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B125">
         <v>1</v>
       </c>
@@ -2545,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B126">
         <v>0</v>
       </c>
@@ -2556,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B127">
         <v>1</v>
       </c>
@@ -2567,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B128">
         <v>1</v>
       </c>
@@ -2578,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B129">
         <v>1</v>
       </c>
@@ -2589,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B130">
         <v>1</v>
       </c>
@@ -2600,7 +2619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B131">
         <v>0</v>
       </c>
@@ -2611,7 +2630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B132">
         <v>0</v>
       </c>
@@ -2622,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B133">
         <v>1</v>
       </c>
@@ -2633,7 +2652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B134">
         <v>1</v>
       </c>
@@ -2644,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B135">
         <v>1</v>
       </c>

</xml_diff>